<commit_message>
Init gestione della comunicazine. Gestita creazione della lobby da parte dell'host e connessione del client alla lobby, messaggio di conferma della creazione.
</commit_message>
<xml_diff>
--- a/LIB_Library/Communication/Messages/MessagesDefinition.xlsx
+++ b/LIB_Library/Communication/Messages/MessagesDefinition.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renny\Documents\GitHub\ArcadeGamesWpf\LIB_Library\Communication\Messages\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5B9421-DA57-4924-9438-9A707A3E6B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,10 +24,85 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>Nome Messaggio</t>
+  </si>
+  <si>
+    <t>Codice</t>
+  </si>
+  <si>
+    <t>Descrizione</t>
+  </si>
+  <si>
+    <t>Tipo*</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>0=&gt;MultiDirezione</t>
+  </si>
+  <si>
+    <t>1=&gt;Host verso client</t>
+  </si>
+  <si>
+    <t>2=&gt;Client verso Host</t>
+  </si>
+  <si>
+    <t>LobbyChatMessage</t>
+  </si>
+  <si>
+    <t>Manda un messggio di testo nella chat della lobby</t>
+  </si>
+  <si>
+    <t>ConnectionConfirmation</t>
+  </si>
+  <si>
+    <t>ConnectionConfirmed</t>
+  </si>
+  <si>
+    <t>Messaggio di prova dal client per verificare la connessione</t>
+  </si>
+  <si>
+    <t>LobbyInfo</t>
+  </si>
+  <si>
+    <t>Messaggio contenent le informazioni della lobby</t>
+  </si>
+  <si>
+    <t>LobbyLogin</t>
+  </si>
+  <si>
+    <t>Messaggio per informare che il client è entrato nella lobby e deve ricevere le informazioni della lobby.</t>
+  </si>
+  <si>
+    <t>Messaggio dell'host per confermare il messaggio del client</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,11 +130,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +413,123 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="28.36328125" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+    <col min="3" max="3" width="113.7265625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="6" max="6" width="24.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1001</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>1002</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>1003</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1004</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C23" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>